<commit_message>
run all for 8760
</commit_message>
<xml_diff>
--- a/network3_input.xlsx
+++ b/network3_input.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcl2\Documents\MATLAB\network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanshan\Documents\GitHub\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="12270" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="12270" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="edge" sheetId="1" r:id="rId1"/>
     <sheet name="node" sheetId="2" r:id="rId2"/>
+    <sheet name="edge (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Edge</t>
   </si>
@@ -423,7 +424,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -657,4 +658,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.1351</v>
+      </c>
+      <c r="C2">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>5.74E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>5.74E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>5.74E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>5.74E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>